<commit_message>
20th April 2nd update
</commit_message>
<xml_diff>
--- a/covid19_data/excel/state/ncov19state_wide.xlsx
+++ b/covid19_data/excel/state/ncov19state_wide.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t xml:space="preserve">detectedstate</t>
   </si>
@@ -131,9 +131,15 @@
     <t xml:space="preserve">19/03/2020</t>
   </si>
   <si>
+    <t xml:space="preserve">19/04/2020</t>
+  </si>
+  <si>
     <t xml:space="preserve">20/03/2020</t>
   </si>
   <si>
+    <t xml:space="preserve">20/04/2020</t>
+  </si>
+  <si>
     <t xml:space="preserve">21/03/2020</t>
   </si>
   <si>
@@ -237,9 +243,6 @@
   </si>
   <si>
     <t xml:space="preserve">Mizoram</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nagaland</t>
   </si>
   <si>
     <t xml:space="preserve">Odisha</t>
@@ -758,10 +761,16 @@
       <c r="AZ1" t="s">
         <v>51</v>
       </c>
+      <c r="BA1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B2"/>
       <c r="C2"/>
@@ -818,10 +827,12 @@
       <c r="AX2"/>
       <c r="AY2"/>
       <c r="AZ2"/>
+      <c r="BA2"/>
+      <c r="BB2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B3"/>
       <c r="C3"/>
@@ -867,31 +878,35 @@
         <v>2</v>
       </c>
       <c r="AM3"/>
-      <c r="AN3"/>
+      <c r="AN3" t="n">
+        <v>1</v>
+      </c>
       <c r="AO3"/>
       <c r="AP3"/>
       <c r="AQ3"/>
       <c r="AR3"/>
       <c r="AS3"/>
-      <c r="AT3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU3" t="n">
+      <c r="AT3"/>
+      <c r="AU3"/>
+      <c r="AV3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW3" t="n">
         <v>5</v>
       </c>
-      <c r="AV3" t="n">
-        <v>3</v>
-      </c>
-      <c r="AW3"/>
-      <c r="AX3"/>
-      <c r="AY3" t="n">
-        <v>1</v>
-      </c>
+      <c r="AX3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AY3"/>
       <c r="AZ3"/>
+      <c r="BA3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B4" t="n">
         <v>67</v>
@@ -971,21 +986,21 @@
       <c r="AM4" t="n">
         <v>2</v>
       </c>
-      <c r="AN4"/>
-      <c r="AO4" t="n">
-        <v>2</v>
-      </c>
+      <c r="AN4" t="n">
+        <v>44</v>
+      </c>
+      <c r="AO4"/>
       <c r="AP4" t="n">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="AQ4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AR4" t="n">
         <v>1</v>
       </c>
       <c r="AS4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT4" t="n">
         <v>1</v>
@@ -994,22 +1009,28 @@
         <v>2</v>
       </c>
       <c r="AV4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AX4" t="n">
         <v>6</v>
       </c>
-      <c r="AW4" t="n">
-        <v>2</v>
-      </c>
-      <c r="AX4"/>
       <c r="AY4" t="n">
         <v>2</v>
       </c>
-      <c r="AZ4" t="n">
+      <c r="AZ4"/>
+      <c r="BA4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BB4" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B5"/>
       <c r="C5"/>
@@ -1064,10 +1085,12 @@
       <c r="AX5"/>
       <c r="AY5"/>
       <c r="AZ5"/>
+      <c r="BA5"/>
+      <c r="BB5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B6" t="n">
         <v>15</v>
@@ -1103,7 +1126,9 @@
       <c r="W6"/>
       <c r="X6"/>
       <c r="Y6"/>
-      <c r="Z6"/>
+      <c r="Z6" t="n">
+        <v>1</v>
+      </c>
       <c r="AA6"/>
       <c r="AB6" t="n">
         <v>2</v>
@@ -1135,13 +1160,15 @@
       <c r="AW6"/>
       <c r="AX6"/>
       <c r="AY6"/>
-      <c r="AZ6" t="n">
+      <c r="AZ6"/>
+      <c r="BA6"/>
+      <c r="BB6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B7" t="n">
         <v>3</v>
@@ -1209,39 +1236,43 @@
         <v>1</v>
       </c>
       <c r="AM7"/>
-      <c r="AN7"/>
+      <c r="AN7" t="n">
+        <v>10</v>
+      </c>
       <c r="AO7"/>
-      <c r="AP7" t="n">
-        <v>2</v>
-      </c>
-      <c r="AQ7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR7"/>
+      <c r="AP7"/>
+      <c r="AQ7"/>
+      <c r="AR7" t="n">
+        <v>2</v>
+      </c>
       <c r="AS7" t="n">
         <v>1</v>
       </c>
-      <c r="AT7" t="n">
-        <v>3</v>
-      </c>
+      <c r="AT7"/>
       <c r="AU7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AV7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AW7" t="n">
+        <v>2</v>
+      </c>
+      <c r="AX7" t="n">
+        <v>2</v>
+      </c>
+      <c r="AY7" t="n">
         <v>4</v>
       </c>
-      <c r="AX7"/>
-      <c r="AY7"/>
-      <c r="AZ7" t="n">
+      <c r="AZ7"/>
+      <c r="BA7"/>
+      <c r="BB7" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B8" t="n">
         <v>2</v>
@@ -1294,34 +1325,38 @@
         <v>1</v>
       </c>
       <c r="AN8" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO8" t="n">
         <v>4</v>
       </c>
-      <c r="AO8"/>
-      <c r="AP8" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ8" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR8"/>
-      <c r="AS8"/>
+      <c r="AP8"/>
+      <c r="AQ8"/>
+      <c r="AR8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS8" t="n">
+        <v>1</v>
+      </c>
       <c r="AT8"/>
-      <c r="AU8" t="n">
-        <v>1</v>
-      </c>
+      <c r="AU8"/>
       <c r="AV8"/>
-      <c r="AW8"/>
+      <c r="AW8" t="n">
+        <v>1</v>
+      </c>
       <c r="AX8"/>
-      <c r="AY8" t="n">
+      <c r="AY8"/>
+      <c r="AZ8"/>
+      <c r="BA8" t="n">
         <v>5</v>
       </c>
-      <c r="AZ8" t="n">
+      <c r="BB8" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B9"/>
       <c r="C9"/>
@@ -1380,28 +1415,30 @@
       <c r="AP9"/>
       <c r="AQ9"/>
       <c r="AR9"/>
-      <c r="AS9" t="n">
-        <v>2</v>
-      </c>
-      <c r="AT9" t="n">
-        <v>3</v>
-      </c>
-      <c r="AU9"/>
+      <c r="AS9"/>
+      <c r="AT9"/>
+      <c r="AU9" t="n">
+        <v>2</v>
+      </c>
       <c r="AV9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AW9"/>
-      <c r="AX9"/>
-      <c r="AY9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ9" t="n">
+      <c r="AX9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY9"/>
+      <c r="AZ9"/>
+      <c r="BA9" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB9" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B10" t="n">
         <v>32</v>
@@ -1498,44 +1535,48 @@
         <v>3</v>
       </c>
       <c r="AN10" t="n">
+        <v>110</v>
+      </c>
+      <c r="AO10" t="n">
         <v>6</v>
       </c>
-      <c r="AO10" t="n">
+      <c r="AP10"/>
+      <c r="AQ10" t="n">
         <v>7</v>
       </c>
-      <c r="AP10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ10" t="n">
-        <v>2</v>
-      </c>
-      <c r="AR10"/>
+      <c r="AR10" t="n">
+        <v>1</v>
+      </c>
       <c r="AS10" t="n">
+        <v>2</v>
+      </c>
+      <c r="AT10"/>
+      <c r="AU10" t="n">
         <v>5</v>
       </c>
-      <c r="AT10" t="n">
+      <c r="AV10" t="n">
         <v>4</v>
       </c>
-      <c r="AU10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV10" t="n">
+      <c r="AW10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX10" t="n">
         <v>9</v>
       </c>
-      <c r="AW10" t="n">
+      <c r="AY10" t="n">
         <v>23</v>
       </c>
-      <c r="AX10"/>
-      <c r="AY10" t="n">
+      <c r="AZ10"/>
+      <c r="BA10" t="n">
         <v>25</v>
       </c>
-      <c r="AZ10" t="n">
+      <c r="BB10" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B11"/>
       <c r="C11"/>
@@ -1584,22 +1625,24 @@
       <c r="AP11"/>
       <c r="AQ11"/>
       <c r="AR11"/>
-      <c r="AS11" t="n">
-        <v>3</v>
-      </c>
+      <c r="AS11"/>
       <c r="AT11"/>
-      <c r="AU11"/>
+      <c r="AU11" t="n">
+        <v>3</v>
+      </c>
       <c r="AV11"/>
-      <c r="AW11" t="n">
-        <v>2</v>
-      </c>
+      <c r="AW11"/>
       <c r="AX11"/>
-      <c r="AY11"/>
+      <c r="AY11" t="n">
+        <v>2</v>
+      </c>
       <c r="AZ11"/>
+      <c r="BA11"/>
+      <c r="BB11"/>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B12" t="n">
         <v>13</v>
@@ -1678,46 +1721,52 @@
         <v>2</v>
       </c>
       <c r="AN12" t="n">
+        <v>367</v>
+      </c>
+      <c r="AO12" t="n">
         <v>5</v>
       </c>
-      <c r="AO12" t="n">
+      <c r="AP12" t="n">
+        <v>108</v>
+      </c>
+      <c r="AQ12" t="n">
         <v>7</v>
       </c>
-      <c r="AP12" t="n">
+      <c r="AR12" t="n">
         <v>4</v>
       </c>
-      <c r="AQ12" t="n">
+      <c r="AS12" t="n">
         <v>12</v>
-      </c>
-      <c r="AR12" t="n">
-        <v>6</v>
-      </c>
-      <c r="AS12" t="n">
-        <v>2</v>
       </c>
       <c r="AT12" t="n">
         <v>6</v>
       </c>
       <c r="AU12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AV12" t="n">
+        <v>6</v>
+      </c>
+      <c r="AW12" t="n">
+        <v>3</v>
+      </c>
+      <c r="AX12" t="n">
         <v>8</v>
       </c>
-      <c r="AW12" t="n">
+      <c r="AY12" t="n">
         <v>8</v>
       </c>
-      <c r="AX12"/>
-      <c r="AY12" t="n">
+      <c r="AZ12"/>
+      <c r="BA12" t="n">
         <v>7</v>
       </c>
-      <c r="AZ12" t="n">
+      <c r="BB12" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B13"/>
       <c r="C13"/>
@@ -1798,42 +1847,48 @@
       </c>
       <c r="AM13"/>
       <c r="AN13" t="n">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="AO13" t="n">
         <v>2</v>
       </c>
-      <c r="AP13"/>
+      <c r="AP13" t="n">
+        <v>1</v>
+      </c>
       <c r="AQ13" t="n">
+        <v>2</v>
+      </c>
+      <c r="AR13"/>
+      <c r="AS13" t="n">
         <v>7</v>
       </c>
-      <c r="AR13" t="n">
-        <v>2</v>
-      </c>
-      <c r="AS13" t="n">
-        <v>1</v>
-      </c>
       <c r="AT13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AU13" t="n">
         <v>1</v>
       </c>
       <c r="AV13" t="n">
-        <v>2</v>
-      </c>
-      <c r="AW13"/>
-      <c r="AX13"/>
-      <c r="AY13" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX13" t="n">
+        <v>2</v>
+      </c>
+      <c r="AY13"/>
+      <c r="AZ13"/>
+      <c r="BA13" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB13" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -1895,16 +1950,16 @@
         <v>1</v>
       </c>
       <c r="AM14"/>
-      <c r="AN14" t="n">
-        <v>2</v>
-      </c>
-      <c r="AO14"/>
+      <c r="AN14"/>
+      <c r="AO14" t="n">
+        <v>2</v>
+      </c>
       <c r="AP14"/>
-      <c r="AQ14" t="n">
-        <v>1</v>
-      </c>
+      <c r="AQ14"/>
       <c r="AR14"/>
-      <c r="AS14"/>
+      <c r="AS14" t="n">
+        <v>1</v>
+      </c>
       <c r="AT14"/>
       <c r="AU14"/>
       <c r="AV14"/>
@@ -1912,10 +1967,12 @@
       <c r="AX14"/>
       <c r="AY14"/>
       <c r="AZ14"/>
+      <c r="BA14"/>
+      <c r="BB14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B15" t="n">
         <v>7</v>
@@ -1999,39 +2056,43 @@
         <v>13</v>
       </c>
       <c r="AM15"/>
-      <c r="AN15"/>
+      <c r="AN15" t="n">
+        <v>13</v>
+      </c>
       <c r="AO15"/>
       <c r="AP15"/>
       <c r="AQ15"/>
-      <c r="AR15" t="n">
-        <v>2</v>
-      </c>
-      <c r="AS15" t="n">
+      <c r="AR15"/>
+      <c r="AS15"/>
+      <c r="AT15" t="n">
+        <v>2</v>
+      </c>
+      <c r="AU15" t="n">
         <v>5</v>
       </c>
-      <c r="AT15" t="n">
-        <v>3</v>
-      </c>
-      <c r="AU15" t="n">
+      <c r="AV15" t="n">
+        <v>3</v>
+      </c>
+      <c r="AW15" t="n">
         <v>6</v>
       </c>
-      <c r="AV15" t="n">
+      <c r="AX15" t="n">
         <v>13</v>
       </c>
-      <c r="AW15" t="n">
+      <c r="AY15" t="n">
         <v>5</v>
       </c>
-      <c r="AX15"/>
-      <c r="AY15" t="n">
+      <c r="AZ15"/>
+      <c r="BA15" t="n">
         <v>11</v>
       </c>
-      <c r="AZ15" t="n">
+      <c r="BB15" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B16"/>
       <c r="C16"/>
@@ -2097,7 +2158,9 @@
         <v>1</v>
       </c>
       <c r="AM16"/>
-      <c r="AN16"/>
+      <c r="AN16" t="n">
+        <v>8</v>
+      </c>
       <c r="AO16"/>
       <c r="AP16"/>
       <c r="AQ16"/>
@@ -2109,13 +2172,15 @@
       <c r="AW16"/>
       <c r="AX16"/>
       <c r="AY16"/>
-      <c r="AZ16" t="n">
+      <c r="AZ16"/>
+      <c r="BA16"/>
+      <c r="BB16" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B17" t="n">
         <v>9</v>
@@ -2207,45 +2272,51 @@
       <c r="AM17" t="n">
         <v>1</v>
       </c>
-      <c r="AN17"/>
-      <c r="AO17" t="n">
+      <c r="AN17" t="n">
+        <v>6</v>
+      </c>
+      <c r="AO17"/>
+      <c r="AP17" t="n">
         <v>5</v>
       </c>
-      <c r="AP17" t="n">
+      <c r="AQ17" t="n">
+        <v>5</v>
+      </c>
+      <c r="AR17" t="n">
         <v>6</v>
       </c>
-      <c r="AQ17" t="n">
+      <c r="AS17" t="n">
         <v>7</v>
       </c>
-      <c r="AR17" t="n">
+      <c r="AT17" t="n">
         <v>8</v>
       </c>
-      <c r="AS17" t="n">
+      <c r="AU17" t="n">
         <v>10</v>
       </c>
-      <c r="AT17" t="n">
+      <c r="AV17" t="n">
         <v>4</v>
       </c>
-      <c r="AU17" t="n">
+      <c r="AW17" t="n">
         <v>9</v>
       </c>
-      <c r="AV17" t="n">
+      <c r="AX17" t="n">
         <v>12</v>
       </c>
-      <c r="AW17" t="n">
+      <c r="AY17" t="n">
         <v>7</v>
       </c>
-      <c r="AX17"/>
-      <c r="AY17" t="n">
+      <c r="AZ17"/>
+      <c r="BA17" t="n">
         <v>5</v>
       </c>
-      <c r="AZ17" t="n">
+      <c r="BB17" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B18" t="n">
         <v>24</v>
@@ -2342,48 +2413,52 @@
         <v>1</v>
       </c>
       <c r="AN18" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="AO18" t="n">
         <v>12</v>
       </c>
-      <c r="AP18" t="n">
+      <c r="AP18"/>
+      <c r="AQ18" t="n">
+        <v>12</v>
+      </c>
+      <c r="AR18" t="n">
         <v>15</v>
       </c>
-      <c r="AQ18" t="n">
+      <c r="AS18" t="n">
         <v>28</v>
       </c>
-      <c r="AR18" t="n">
+      <c r="AT18" t="n">
         <v>14</v>
       </c>
-      <c r="AS18" t="n">
+      <c r="AU18" t="n">
         <v>9</v>
       </c>
-      <c r="AT18" t="n">
+      <c r="AV18" t="n">
         <v>19</v>
       </c>
-      <c r="AU18" t="n">
+      <c r="AW18" t="n">
         <v>39</v>
       </c>
-      <c r="AV18" t="n">
+      <c r="AX18" t="n">
         <v>6</v>
       </c>
-      <c r="AW18" t="n">
+      <c r="AY18" t="n">
         <v>20</v>
       </c>
-      <c r="AX18" t="n">
-        <v>1</v>
-      </c>
-      <c r="AY18" t="n">
+      <c r="AZ18" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA18" t="n">
         <v>32</v>
       </c>
-      <c r="AZ18" t="n">
+      <c r="BB18" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B19"/>
       <c r="C19"/>
@@ -2437,14 +2512,14 @@
       <c r="AK19"/>
       <c r="AL19"/>
       <c r="AM19"/>
-      <c r="AN19" t="n">
-        <v>2</v>
-      </c>
+      <c r="AN19"/>
       <c r="AO19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AP19"/>
-      <c r="AQ19"/>
+      <c r="AQ19" t="n">
+        <v>3</v>
+      </c>
       <c r="AR19"/>
       <c r="AS19"/>
       <c r="AT19"/>
@@ -2454,10 +2529,12 @@
       <c r="AX19"/>
       <c r="AY19"/>
       <c r="AZ19"/>
+      <c r="BA19"/>
+      <c r="BB19"/>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B20" t="n">
         <v>32</v>
@@ -2534,40 +2611,44 @@
       </c>
       <c r="AM20"/>
       <c r="AN20" t="n">
+        <v>5</v>
+      </c>
+      <c r="AO20" t="n">
         <v>4</v>
       </c>
-      <c r="AO20"/>
-      <c r="AP20" t="n">
-        <v>2</v>
-      </c>
+      <c r="AP20"/>
       <c r="AQ20"/>
       <c r="AR20" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS20" t="n">
+        <v>2</v>
+      </c>
+      <c r="AS20"/>
+      <c r="AT20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU20" t="n">
         <v>8</v>
       </c>
-      <c r="AT20" t="n">
+      <c r="AV20" t="n">
         <v>5</v>
       </c>
-      <c r="AU20" t="n">
+      <c r="AW20" t="n">
         <v>9</v>
       </c>
-      <c r="AV20" t="n">
+      <c r="AX20" t="n">
         <v>10</v>
       </c>
-      <c r="AW20"/>
-      <c r="AX20"/>
-      <c r="AY20" t="n">
+      <c r="AY20"/>
+      <c r="AZ20"/>
+      <c r="BA20" t="n">
         <v>8</v>
       </c>
-      <c r="AZ20" t="n">
+      <c r="BB20" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B21" t="n">
         <v>33</v>
@@ -2636,76 +2717,82 @@
         <v>9</v>
       </c>
       <c r="AD21" t="n">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="AE21" t="n">
         <v>6</v>
       </c>
       <c r="AF21" t="n">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="AG21" t="n">
         <v>7</v>
       </c>
       <c r="AH21" t="n">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AI21" t="n">
         <v>2</v>
       </c>
       <c r="AJ21" t="n">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="AK21" t="n">
         <v>4</v>
       </c>
       <c r="AL21" t="n">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AM21" t="n">
         <v>3</v>
       </c>
       <c r="AN21" t="n">
+        <v>552</v>
+      </c>
+      <c r="AO21" t="n">
         <v>4</v>
       </c>
-      <c r="AO21" t="n">
+      <c r="AP21" t="n">
+        <v>283</v>
+      </c>
+      <c r="AQ21" t="n">
         <v>12</v>
       </c>
-      <c r="AP21" t="n">
+      <c r="AR21" t="n">
         <v>10</v>
-      </c>
-      <c r="AQ21" t="n">
-        <v>15</v>
-      </c>
-      <c r="AR21" t="n">
-        <v>18</v>
       </c>
       <c r="AS21" t="n">
         <v>15</v>
       </c>
       <c r="AT21" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="AU21" t="n">
+        <v>15</v>
+      </c>
+      <c r="AV21" t="n">
+        <v>3</v>
+      </c>
+      <c r="AW21" t="n">
         <v>28</v>
       </c>
-      <c r="AV21" t="n">
+      <c r="AX21" t="n">
         <v>28</v>
       </c>
-      <c r="AW21" t="n">
+      <c r="AY21" t="n">
         <v>22</v>
       </c>
-      <c r="AX21"/>
-      <c r="AY21" t="n">
+      <c r="AZ21"/>
+      <c r="BA21" t="n">
         <v>17</v>
       </c>
-      <c r="AZ21" t="n">
+      <c r="BB21" t="n">
         <v>82</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B22"/>
       <c r="C22"/>
@@ -2751,21 +2838,23 @@
       <c r="AO22"/>
       <c r="AP22"/>
       <c r="AQ22"/>
-      <c r="AR22" t="n">
-        <v>1</v>
-      </c>
+      <c r="AR22"/>
       <c r="AS22"/>
-      <c r="AT22"/>
+      <c r="AT22" t="n">
+        <v>1</v>
+      </c>
       <c r="AU22"/>
       <c r="AV22"/>
       <c r="AW22"/>
       <c r="AX22"/>
       <c r="AY22"/>
       <c r="AZ22"/>
+      <c r="BA22"/>
+      <c r="BB22"/>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B23"/>
       <c r="C23"/>
@@ -2826,10 +2915,12 @@
       <c r="AX23"/>
       <c r="AY23"/>
       <c r="AZ23"/>
+      <c r="BA23"/>
+      <c r="BB23"/>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B24"/>
       <c r="C24"/>
@@ -2874,1100 +2965,1084 @@
       <c r="AP24"/>
       <c r="AQ24"/>
       <c r="AR24"/>
-      <c r="AS24" t="n">
-        <v>1</v>
-      </c>
+      <c r="AS24"/>
       <c r="AT24"/>
-      <c r="AU24"/>
+      <c r="AU24" t="n">
+        <v>1</v>
+      </c>
       <c r="AV24"/>
       <c r="AW24"/>
       <c r="AX24"/>
       <c r="AY24"/>
       <c r="AZ24"/>
+      <c r="BA24"/>
+      <c r="BB24"/>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>75</v>
-      </c>
-      <c r="B25"/>
+        <v>77</v>
+      </c>
+      <c r="B25" t="n">
+        <v>1</v>
+      </c>
       <c r="C25"/>
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25"/>
       <c r="G25"/>
-      <c r="H25"/>
+      <c r="H25" t="n">
+        <v>15</v>
+      </c>
       <c r="I25"/>
-      <c r="J25"/>
+      <c r="J25" t="n">
+        <v>1</v>
+      </c>
       <c r="K25"/>
-      <c r="L25"/>
+      <c r="L25" t="n">
+        <v>18</v>
+      </c>
       <c r="M25"/>
-      <c r="N25"/>
+      <c r="N25" t="n">
+        <v>1</v>
+      </c>
       <c r="O25"/>
-      <c r="P25"/>
+      <c r="P25" t="n">
+        <v>2</v>
+      </c>
       <c r="Q25"/>
       <c r="R25"/>
       <c r="S25"/>
-      <c r="T25"/>
+      <c r="T25" t="n">
+        <v>6</v>
+      </c>
       <c r="U25"/>
-      <c r="V25"/>
+      <c r="V25" t="n">
+        <v>2</v>
+      </c>
       <c r="W25"/>
-      <c r="X25"/>
+      <c r="X25" t="n">
+        <v>4</v>
+      </c>
       <c r="Y25"/>
-      <c r="Z25" t="n">
-        <v>1</v>
-      </c>
+      <c r="Z25"/>
       <c r="AA25"/>
-      <c r="AB25"/>
+      <c r="AB25" t="n">
+        <v>1</v>
+      </c>
       <c r="AC25"/>
-      <c r="AD25"/>
+      <c r="AD25" t="n">
+        <v>5</v>
+      </c>
       <c r="AE25"/>
       <c r="AF25"/>
-      <c r="AG25"/>
+      <c r="AG25" t="n">
+        <v>1</v>
+      </c>
       <c r="AH25"/>
       <c r="AI25"/>
       <c r="AJ25"/>
       <c r="AK25"/>
-      <c r="AL25"/>
-      <c r="AM25"/>
+      <c r="AL25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM25" t="n">
+        <v>1</v>
+      </c>
       <c r="AN25"/>
       <c r="AO25"/>
-      <c r="AP25"/>
+      <c r="AP25" t="n">
+        <v>12</v>
+      </c>
       <c r="AQ25"/>
       <c r="AR25"/>
       <c r="AS25"/>
       <c r="AT25"/>
       <c r="AU25"/>
-      <c r="AV25"/>
+      <c r="AV25" t="n">
+        <v>1</v>
+      </c>
       <c r="AW25"/>
       <c r="AX25"/>
       <c r="AY25"/>
       <c r="AZ25"/>
+      <c r="BA25"/>
+      <c r="BB25" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C26"/>
       <c r="D26"/>
-      <c r="E26"/>
+      <c r="E26" t="n">
+        <v>2</v>
+      </c>
       <c r="F26"/>
       <c r="G26"/>
-      <c r="H26" t="n">
-        <v>15</v>
-      </c>
+      <c r="H26"/>
       <c r="I26"/>
-      <c r="J26" t="n">
-        <v>1</v>
-      </c>
+      <c r="J26"/>
       <c r="K26"/>
-      <c r="L26" t="n">
-        <v>18</v>
-      </c>
+      <c r="L26"/>
       <c r="M26"/>
-      <c r="N26" t="n">
-        <v>1</v>
-      </c>
+      <c r="N26"/>
       <c r="O26"/>
-      <c r="P26" t="n">
-        <v>2</v>
-      </c>
+      <c r="P26"/>
       <c r="Q26"/>
       <c r="R26"/>
       <c r="S26"/>
-      <c r="T26" t="n">
-        <v>6</v>
-      </c>
+      <c r="T26"/>
       <c r="U26"/>
       <c r="V26" t="n">
         <v>2</v>
       </c>
       <c r="W26"/>
-      <c r="X26" t="n">
-        <v>4</v>
-      </c>
+      <c r="X26"/>
       <c r="Y26"/>
       <c r="Z26"/>
       <c r="AA26"/>
-      <c r="AB26" t="n">
-        <v>1</v>
-      </c>
+      <c r="AB26"/>
       <c r="AC26"/>
-      <c r="AD26" t="n">
-        <v>5</v>
-      </c>
+      <c r="AD26"/>
       <c r="AE26"/>
       <c r="AF26"/>
-      <c r="AG26" t="n">
-        <v>1</v>
-      </c>
+      <c r="AG26"/>
       <c r="AH26"/>
-      <c r="AI26"/>
+      <c r="AI26" t="n">
+        <v>1</v>
+      </c>
       <c r="AJ26"/>
       <c r="AK26"/>
-      <c r="AL26" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM26" t="n">
-        <v>1</v>
-      </c>
+      <c r="AL26"/>
+      <c r="AM26"/>
       <c r="AN26"/>
       <c r="AO26"/>
       <c r="AP26"/>
       <c r="AQ26"/>
       <c r="AR26"/>
       <c r="AS26"/>
-      <c r="AT26" t="n">
-        <v>1</v>
-      </c>
+      <c r="AT26"/>
       <c r="AU26"/>
       <c r="AV26"/>
       <c r="AW26"/>
       <c r="AX26"/>
       <c r="AY26"/>
-      <c r="AZ26" t="n">
-        <v>1</v>
-      </c>
+      <c r="AZ26"/>
+      <c r="BA26"/>
+      <c r="BB26"/>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B27" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27"/>
       <c r="G27"/>
-      <c r="H27"/>
+      <c r="H27" t="n">
+        <v>6</v>
+      </c>
       <c r="I27"/>
-      <c r="J27"/>
+      <c r="J27" t="n">
+        <v>12</v>
+      </c>
       <c r="K27"/>
-      <c r="L27"/>
+      <c r="L27" t="n">
+        <v>3</v>
+      </c>
       <c r="M27"/>
-      <c r="N27"/>
+      <c r="N27" t="n">
+        <v>11</v>
+      </c>
       <c r="O27"/>
-      <c r="P27"/>
+      <c r="P27" t="n">
+        <v>20</v>
+      </c>
       <c r="Q27"/>
-      <c r="R27"/>
-      <c r="S27"/>
-      <c r="T27"/>
+      <c r="R27" t="n">
+        <v>7</v>
+      </c>
+      <c r="S27" t="n">
+        <v>1</v>
+      </c>
+      <c r="T27" t="n">
+        <v>24</v>
+      </c>
       <c r="U27"/>
       <c r="V27" t="n">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="W27"/>
-      <c r="X27"/>
+      <c r="X27" t="n">
+        <v>7</v>
+      </c>
       <c r="Y27"/>
-      <c r="Z27"/>
+      <c r="Z27" t="n">
+        <v>12</v>
+      </c>
       <c r="AA27"/>
-      <c r="AB27"/>
+      <c r="AB27" t="n">
+        <v>6</v>
+      </c>
       <c r="AC27"/>
-      <c r="AD27"/>
+      <c r="AD27" t="n">
+        <v>8</v>
+      </c>
       <c r="AE27"/>
-      <c r="AF27"/>
+      <c r="AF27" t="n">
+        <v>2</v>
+      </c>
       <c r="AG27"/>
-      <c r="AH27"/>
-      <c r="AI27" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ27"/>
+      <c r="AH27" t="n">
+        <v>11</v>
+      </c>
+      <c r="AI27"/>
+      <c r="AJ27" t="n">
+        <v>14</v>
+      </c>
       <c r="AK27"/>
-      <c r="AL27"/>
-      <c r="AM27"/>
-      <c r="AN27"/>
-      <c r="AO27"/>
+      <c r="AL27" t="n">
+        <v>23</v>
+      </c>
+      <c r="AM27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN27" t="n">
+        <v>10</v>
+      </c>
+      <c r="AO27" t="n">
+        <v>1</v>
+      </c>
       <c r="AP27"/>
-      <c r="AQ27"/>
-      <c r="AR27"/>
-      <c r="AS27"/>
-      <c r="AT27"/>
-      <c r="AU27"/>
-      <c r="AV27"/>
-      <c r="AW27"/>
+      <c r="AQ27" t="n">
+        <v>10</v>
+      </c>
+      <c r="AR27" t="n">
+        <v>8</v>
+      </c>
+      <c r="AS27" t="n">
+        <v>2</v>
+      </c>
+      <c r="AT27" t="n">
+        <v>6</v>
+      </c>
+      <c r="AU27" t="n">
+        <v>2</v>
+      </c>
+      <c r="AV27" t="n">
+        <v>2</v>
+      </c>
+      <c r="AW27" t="n">
+        <v>5</v>
+      </c>
       <c r="AX27"/>
       <c r="AY27"/>
       <c r="AZ27"/>
+      <c r="BA27" t="n">
+        <v>3</v>
+      </c>
+      <c r="BB27" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B28" t="n">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="F28"/>
-      <c r="G28"/>
+      <c r="G28" t="n">
+        <v>1</v>
+      </c>
       <c r="H28" t="n">
-        <v>6</v>
-      </c>
-      <c r="I28"/>
+        <v>46</v>
+      </c>
+      <c r="I28" t="n">
+        <v>1</v>
+      </c>
       <c r="J28" t="n">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="K28"/>
       <c r="L28" t="n">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="M28"/>
       <c r="N28" t="n">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="O28"/>
       <c r="P28" t="n">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="Q28"/>
       <c r="R28" t="n">
-        <v>7</v>
-      </c>
-      <c r="S28" t="n">
-        <v>1</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="S28"/>
       <c r="T28" t="n">
-        <v>24</v>
-      </c>
-      <c r="U28"/>
+        <v>80</v>
+      </c>
+      <c r="U28" t="n">
+        <v>1</v>
+      </c>
       <c r="V28" t="n">
-        <v>21</v>
+        <v>98</v>
       </c>
       <c r="W28"/>
       <c r="X28" t="n">
-        <v>7</v>
+        <v>139</v>
       </c>
       <c r="Y28"/>
       <c r="Z28" t="n">
-        <v>12</v>
+        <v>104</v>
       </c>
       <c r="AA28"/>
       <c r="AB28" t="n">
-        <v>6</v>
-      </c>
-      <c r="AC28"/>
+        <v>93</v>
+      </c>
+      <c r="AC28" t="n">
+        <v>1</v>
+      </c>
       <c r="AD28" t="n">
-        <v>8</v>
+        <v>108</v>
       </c>
       <c r="AE28"/>
       <c r="AF28" t="n">
-        <v>2</v>
+        <v>71</v>
       </c>
       <c r="AG28"/>
       <c r="AH28" t="n">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="AI28"/>
       <c r="AJ28" t="n">
+        <v>98</v>
+      </c>
+      <c r="AK28" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL28" t="n">
+        <v>122</v>
+      </c>
+      <c r="AM28" t="n">
+        <v>2</v>
+      </c>
+      <c r="AN28" t="n">
+        <v>127</v>
+      </c>
+      <c r="AO28" t="n">
+        <v>8</v>
+      </c>
+      <c r="AP28" t="n">
+        <v>57</v>
+      </c>
+      <c r="AQ28" t="n">
+        <v>7</v>
+      </c>
+      <c r="AR28" t="n">
+        <v>5</v>
+      </c>
+      <c r="AS28" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT28"/>
+      <c r="AU28" t="n">
+        <v>6</v>
+      </c>
+      <c r="AV28" t="n">
+        <v>5</v>
+      </c>
+      <c r="AW28" t="n">
+        <v>7</v>
+      </c>
+      <c r="AX28" t="n">
+        <v>4</v>
+      </c>
+      <c r="AY28" t="n">
+        <v>5</v>
+      </c>
+      <c r="AZ28"/>
+      <c r="BA28" t="n">
+        <v>20</v>
+      </c>
+      <c r="BB28" t="n">
         <v>14</v>
-      </c>
-      <c r="AK28"/>
-      <c r="AL28" t="n">
-        <v>23</v>
-      </c>
-      <c r="AM28" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN28" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO28" t="n">
-        <v>10</v>
-      </c>
-      <c r="AP28" t="n">
-        <v>8</v>
-      </c>
-      <c r="AQ28" t="n">
-        <v>2</v>
-      </c>
-      <c r="AR28" t="n">
-        <v>6</v>
-      </c>
-      <c r="AS28" t="n">
-        <v>2</v>
-      </c>
-      <c r="AT28" t="n">
-        <v>2</v>
-      </c>
-      <c r="AU28" t="n">
-        <v>5</v>
-      </c>
-      <c r="AV28"/>
-      <c r="AW28"/>
-      <c r="AX28"/>
-      <c r="AY28" t="n">
-        <v>3</v>
-      </c>
-      <c r="AZ28" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B29" t="n">
-        <v>27</v>
+        <v>110</v>
       </c>
       <c r="C29"/>
       <c r="D29"/>
       <c r="E29" t="n">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="F29"/>
-      <c r="G29" t="n">
-        <v>1</v>
-      </c>
+      <c r="G29"/>
       <c r="H29" t="n">
-        <v>46</v>
-      </c>
-      <c r="I29" t="n">
-        <v>1</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="I29"/>
       <c r="J29" t="n">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="K29"/>
       <c r="L29" t="n">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="M29"/>
       <c r="N29" t="n">
-        <v>35</v>
-      </c>
-      <c r="O29"/>
+        <v>50</v>
+      </c>
+      <c r="O29" t="n">
+        <v>1</v>
+      </c>
       <c r="P29" t="n">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="Q29"/>
       <c r="R29" t="n">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="S29"/>
       <c r="T29" t="n">
-        <v>80</v>
-      </c>
-      <c r="U29" t="n">
-        <v>1</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="U29"/>
       <c r="V29" t="n">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="W29"/>
       <c r="X29" t="n">
-        <v>139</v>
+        <v>58</v>
       </c>
       <c r="Y29"/>
       <c r="Z29" t="n">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="AA29"/>
       <c r="AB29" t="n">
-        <v>93</v>
-      </c>
-      <c r="AC29" t="n">
-        <v>1</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="AC29"/>
       <c r="AD29" t="n">
-        <v>108</v>
+        <v>31</v>
       </c>
       <c r="AE29"/>
       <c r="AF29" t="n">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="AG29"/>
       <c r="AH29" t="n">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="AI29"/>
       <c r="AJ29" t="n">
-        <v>98</v>
+        <v>56</v>
       </c>
       <c r="AK29" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AL29" t="n">
-        <v>122</v>
+        <v>49</v>
       </c>
       <c r="AM29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN29" t="n">
+        <v>105</v>
+      </c>
+      <c r="AO29"/>
+      <c r="AP29"/>
+      <c r="AQ29" t="n">
+        <v>3</v>
+      </c>
+      <c r="AR29" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS29" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT29" t="n">
+        <v>6</v>
+      </c>
+      <c r="AU29" t="n">
         <v>8</v>
       </c>
-      <c r="AO29" t="n">
-        <v>7</v>
-      </c>
-      <c r="AP29" t="n">
-        <v>5</v>
-      </c>
-      <c r="AQ29" t="n">
-        <v>3</v>
-      </c>
-      <c r="AR29"/>
-      <c r="AS29" t="n">
-        <v>6</v>
-      </c>
-      <c r="AT29" t="n">
-        <v>5</v>
-      </c>
-      <c r="AU29" t="n">
-        <v>7</v>
-      </c>
       <c r="AV29" t="n">
+        <v>3</v>
+      </c>
+      <c r="AW29" t="n">
+        <v>9</v>
+      </c>
+      <c r="AX29" t="n">
         <v>4</v>
       </c>
-      <c r="AW29" t="n">
-        <v>5</v>
-      </c>
-      <c r="AX29"/>
       <c r="AY29" t="n">
-        <v>20</v>
-      </c>
-      <c r="AZ29" t="n">
-        <v>14</v>
+        <v>8</v>
+      </c>
+      <c r="AZ29"/>
+      <c r="BA29" t="n">
+        <v>17</v>
+      </c>
+      <c r="BB29" t="n">
+        <v>57</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B30" t="n">
-        <v>110</v>
+        <v>30</v>
       </c>
       <c r="C30"/>
-      <c r="D30"/>
+      <c r="D30" t="n">
+        <v>1</v>
+      </c>
       <c r="E30" t="n">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="F30"/>
       <c r="G30"/>
       <c r="H30" t="n">
-        <v>102</v>
+        <v>75</v>
       </c>
       <c r="I30"/>
       <c r="J30" t="n">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="K30"/>
       <c r="L30" t="n">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="M30"/>
       <c r="N30" t="n">
-        <v>50</v>
-      </c>
-      <c r="O30" t="n">
-        <v>1</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="O30"/>
       <c r="P30" t="n">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="Q30"/>
       <c r="R30" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="S30"/>
       <c r="T30" t="n">
-        <v>96</v>
+        <v>18</v>
       </c>
       <c r="U30"/>
       <c r="V30" t="n">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="W30"/>
       <c r="X30" t="n">
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="Y30"/>
       <c r="Z30" t="n">
-        <v>106</v>
+        <v>28</v>
       </c>
       <c r="AA30"/>
       <c r="AB30" t="n">
-        <v>98</v>
-      </c>
-      <c r="AC30"/>
+        <v>61</v>
+      </c>
+      <c r="AC30" t="n">
+        <v>1</v>
+      </c>
       <c r="AD30" t="n">
-        <v>31</v>
-      </c>
-      <c r="AE30"/>
+        <v>52</v>
+      </c>
+      <c r="AE30" t="n">
+        <v>1</v>
+      </c>
       <c r="AF30" t="n">
-        <v>38</v>
-      </c>
-      <c r="AG30"/>
+        <v>6</v>
+      </c>
+      <c r="AG30" t="n">
+        <v>1</v>
+      </c>
       <c r="AH30" t="n">
-        <v>25</v>
-      </c>
-      <c r="AI30"/>
+        <v>50</v>
+      </c>
+      <c r="AI30" t="n">
+        <v>1</v>
+      </c>
       <c r="AJ30" t="n">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="AK30" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="AL30" t="n">
+        <v>43</v>
+      </c>
+      <c r="AM30" t="n">
+        <v>3</v>
+      </c>
+      <c r="AN30" t="n">
         <v>49</v>
       </c>
-      <c r="AM30" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN30"/>
       <c r="AO30" t="n">
         <v>3</v>
       </c>
-      <c r="AP30" t="n">
-        <v>3</v>
-      </c>
+      <c r="AP30"/>
       <c r="AQ30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AR30" t="n">
         <v>6</v>
       </c>
       <c r="AS30" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="AT30" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AU30" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="AV30" t="n">
         <v>4</v>
       </c>
       <c r="AW30" t="n">
+        <v>14</v>
+      </c>
+      <c r="AX30" t="n">
         <v>8</v>
       </c>
-      <c r="AX30"/>
       <c r="AY30" t="n">
-        <v>17</v>
-      </c>
-      <c r="AZ30" t="n">
-        <v>57</v>
+        <v>3</v>
+      </c>
+      <c r="AZ30"/>
+      <c r="BA30" t="n">
+        <v>7</v>
+      </c>
+      <c r="BB30" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>81</v>
-      </c>
-      <c r="B31" t="n">
-        <v>30</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="B31"/>
       <c r="C31"/>
-      <c r="D31" t="n">
-        <v>1</v>
-      </c>
-      <c r="E31" t="n">
-        <v>27</v>
-      </c>
+      <c r="D31"/>
+      <c r="E31"/>
       <c r="F31"/>
       <c r="G31"/>
-      <c r="H31" t="n">
-        <v>75</v>
-      </c>
+      <c r="H31"/>
       <c r="I31"/>
-      <c r="J31" t="n">
-        <v>43</v>
-      </c>
+      <c r="J31"/>
       <c r="K31"/>
-      <c r="L31" t="n">
-        <v>62</v>
-      </c>
+      <c r="L31"/>
       <c r="M31"/>
       <c r="N31" t="n">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="O31"/>
-      <c r="P31" t="n">
-        <v>40</v>
-      </c>
+      <c r="P31"/>
       <c r="Q31"/>
-      <c r="R31" t="n">
-        <v>49</v>
-      </c>
+      <c r="R31"/>
       <c r="S31"/>
-      <c r="T31" t="n">
-        <v>18</v>
-      </c>
+      <c r="T31"/>
       <c r="U31"/>
       <c r="V31" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="W31"/>
-      <c r="X31" t="n">
-        <v>16</v>
-      </c>
+      <c r="X31"/>
       <c r="Y31"/>
-      <c r="Z31" t="n">
-        <v>28</v>
-      </c>
+      <c r="Z31"/>
       <c r="AA31"/>
-      <c r="AB31" t="n">
-        <v>61</v>
-      </c>
-      <c r="AC31" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD31" t="n">
-        <v>52</v>
-      </c>
-      <c r="AE31" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF31" t="n">
-        <v>6</v>
-      </c>
-      <c r="AG31" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH31" t="n">
-        <v>50</v>
-      </c>
-      <c r="AI31" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ31" t="n">
-        <v>66</v>
-      </c>
-      <c r="AK31" t="n">
-        <v>8</v>
-      </c>
-      <c r="AL31" t="n">
-        <v>43</v>
-      </c>
-      <c r="AM31" t="n">
-        <v>3</v>
-      </c>
-      <c r="AN31" t="n">
-        <v>3</v>
-      </c>
-      <c r="AO31" t="n">
-        <v>2</v>
-      </c>
-      <c r="AP31" t="n">
-        <v>6</v>
-      </c>
-      <c r="AQ31" t="n">
-        <v>6</v>
-      </c>
-      <c r="AR31" t="n">
-        <v>6</v>
-      </c>
-      <c r="AS31" t="n">
-        <v>2</v>
-      </c>
-      <c r="AT31" t="n">
-        <v>4</v>
-      </c>
-      <c r="AU31" t="n">
-        <v>14</v>
-      </c>
-      <c r="AV31" t="n">
-        <v>8</v>
-      </c>
-      <c r="AW31" t="n">
-        <v>3</v>
-      </c>
+      <c r="AB31"/>
+      <c r="AC31"/>
+      <c r="AD31"/>
+      <c r="AE31"/>
+      <c r="AF31"/>
+      <c r="AG31"/>
+      <c r="AH31"/>
+      <c r="AI31"/>
+      <c r="AJ31"/>
+      <c r="AK31"/>
+      <c r="AL31"/>
+      <c r="AM31"/>
+      <c r="AN31"/>
+      <c r="AO31"/>
+      <c r="AP31"/>
+      <c r="AQ31"/>
+      <c r="AR31"/>
+      <c r="AS31"/>
+      <c r="AT31"/>
+      <c r="AU31"/>
+      <c r="AV31"/>
+      <c r="AW31"/>
       <c r="AX31"/>
-      <c r="AY31" t="n">
-        <v>7</v>
-      </c>
-      <c r="AZ31" t="n">
-        <v>20</v>
-      </c>
+      <c r="AY31"/>
+      <c r="AZ31"/>
+      <c r="BA31"/>
+      <c r="BB31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>82</v>
-      </c>
-      <c r="B32"/>
+        <v>84</v>
+      </c>
+      <c r="B32" t="n">
+        <v>13</v>
+      </c>
       <c r="C32"/>
       <c r="D32"/>
-      <c r="E32"/>
+      <c r="E32" t="n">
+        <v>11</v>
+      </c>
       <c r="F32"/>
       <c r="G32"/>
-      <c r="H32"/>
-      <c r="I32"/>
-      <c r="J32"/>
-      <c r="K32"/>
-      <c r="L32"/>
+      <c r="H32" t="n">
+        <v>46</v>
+      </c>
+      <c r="I32" t="n">
+        <v>7</v>
+      </c>
+      <c r="J32" t="n">
+        <v>60</v>
+      </c>
+      <c r="K32" t="n">
+        <v>1</v>
+      </c>
+      <c r="L32" t="n">
+        <v>44</v>
+      </c>
       <c r="M32"/>
       <c r="N32" t="n">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="O32"/>
-      <c r="P32"/>
+      <c r="P32" t="n">
+        <v>27</v>
+      </c>
       <c r="Q32"/>
-      <c r="R32"/>
-      <c r="S32"/>
-      <c r="T32"/>
+      <c r="R32" t="n">
+        <v>29</v>
+      </c>
+      <c r="S32" t="n">
+        <v>2</v>
+      </c>
+      <c r="T32" t="n">
+        <v>49</v>
+      </c>
       <c r="U32"/>
       <c r="V32" t="n">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="W32"/>
-      <c r="X32"/>
-      <c r="Y32"/>
-      <c r="Z32"/>
-      <c r="AA32"/>
-      <c r="AB32"/>
+      <c r="X32" t="n">
+        <v>19</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>31</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB32" t="n">
+        <v>75</v>
+      </c>
       <c r="AC32"/>
-      <c r="AD32"/>
+      <c r="AD32" t="n">
+        <v>102</v>
+      </c>
       <c r="AE32"/>
-      <c r="AF32"/>
+      <c r="AF32" t="n">
+        <v>75</v>
+      </c>
       <c r="AG32"/>
-      <c r="AH32"/>
-      <c r="AI32"/>
-      <c r="AJ32"/>
-      <c r="AK32"/>
-      <c r="AL32"/>
-      <c r="AM32"/>
-      <c r="AN32"/>
-      <c r="AO32"/>
+      <c r="AH32" t="n">
+        <v>70</v>
+      </c>
+      <c r="AI32" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ32" t="n">
+        <v>44</v>
+      </c>
+      <c r="AK32" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL32" t="n">
+        <v>126</v>
+      </c>
+      <c r="AM32" t="n">
+        <v>3</v>
+      </c>
+      <c r="AN32" t="n">
+        <v>125</v>
+      </c>
+      <c r="AO32" t="n">
+        <v>4</v>
+      </c>
       <c r="AP32"/>
-      <c r="AQ32"/>
-      <c r="AR32"/>
-      <c r="AS32"/>
-      <c r="AT32"/>
-      <c r="AU32"/>
-      <c r="AV32"/>
-      <c r="AW32"/>
-      <c r="AX32"/>
-      <c r="AY32"/>
+      <c r="AQ32" t="n">
+        <v>4</v>
+      </c>
+      <c r="AR32" t="n">
+        <v>2</v>
+      </c>
+      <c r="AS32" t="n">
+        <v>4</v>
+      </c>
+      <c r="AT32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU32" t="n">
+        <v>3</v>
+      </c>
+      <c r="AV32" t="n">
+        <v>4</v>
+      </c>
+      <c r="AW32" t="n">
+        <v>7</v>
+      </c>
+      <c r="AX32" t="n">
+        <v>16</v>
+      </c>
+      <c r="AY32" t="n">
+        <v>7</v>
+      </c>
       <c r="AZ32"/>
+      <c r="BA32" t="n">
+        <v>24</v>
+      </c>
+      <c r="BB32" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>83</v>
-      </c>
-      <c r="B33" t="n">
-        <v>13</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="B33"/>
       <c r="C33"/>
       <c r="D33"/>
       <c r="E33" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F33"/>
       <c r="G33"/>
       <c r="H33" t="n">
-        <v>46</v>
-      </c>
-      <c r="I33" t="n">
-        <v>7</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="I33"/>
       <c r="J33" t="n">
-        <v>60</v>
-      </c>
-      <c r="K33" t="n">
-        <v>1</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="K33"/>
       <c r="L33" t="n">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="M33"/>
       <c r="N33" t="n">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="O33"/>
-      <c r="P33" t="n">
-        <v>27</v>
-      </c>
+      <c r="P33"/>
       <c r="Q33"/>
       <c r="R33" t="n">
-        <v>29</v>
-      </c>
-      <c r="S33" t="n">
-        <v>2</v>
-      </c>
-      <c r="T33" t="n">
-        <v>49</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="S33"/>
+      <c r="T33"/>
       <c r="U33"/>
-      <c r="V33" t="n">
-        <v>23</v>
-      </c>
+      <c r="V33"/>
       <c r="W33"/>
-      <c r="X33" t="n">
-        <v>19</v>
-      </c>
-      <c r="Y33" t="n">
-        <v>2</v>
-      </c>
-      <c r="Z33" t="n">
-        <v>31</v>
-      </c>
-      <c r="AA33" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB33" t="n">
-        <v>75</v>
-      </c>
+      <c r="X33"/>
+      <c r="Y33"/>
+      <c r="Z33"/>
+      <c r="AA33"/>
+      <c r="AB33"/>
       <c r="AC33"/>
       <c r="AD33" t="n">
-        <v>102</v>
-      </c>
-      <c r="AE33"/>
-      <c r="AF33" t="n">
-        <v>75</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AE33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF33"/>
       <c r="AG33"/>
-      <c r="AH33" t="n">
-        <v>70</v>
-      </c>
-      <c r="AI33" t="n">
-        <v>2</v>
-      </c>
+      <c r="AH33"/>
+      <c r="AI33"/>
       <c r="AJ33" t="n">
-        <v>44</v>
-      </c>
-      <c r="AK33" t="n">
-        <v>2</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="AK33"/>
       <c r="AL33" t="n">
-        <v>125</v>
+        <v>2</v>
       </c>
       <c r="AM33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AN33" t="n">
-        <v>4</v>
-      </c>
-      <c r="AO33" t="n">
-        <v>4</v>
-      </c>
-      <c r="AP33" t="n">
-        <v>2</v>
-      </c>
-      <c r="AQ33" t="n">
-        <v>4</v>
-      </c>
-      <c r="AR33" t="n">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AO33"/>
+      <c r="AP33"/>
+      <c r="AQ33"/>
+      <c r="AR33"/>
       <c r="AS33" t="n">
-        <v>3</v>
-      </c>
-      <c r="AT33" t="n">
-        <v>4</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AT33"/>
       <c r="AU33" t="n">
-        <v>7</v>
-      </c>
-      <c r="AV33" t="n">
-        <v>16</v>
-      </c>
-      <c r="AW33" t="n">
-        <v>7</v>
-      </c>
-      <c r="AX33"/>
+        <v>1</v>
+      </c>
+      <c r="AV33"/>
+      <c r="AW33"/>
+      <c r="AX33" t="n">
+        <v>1</v>
+      </c>
       <c r="AY33" t="n">
-        <v>24</v>
-      </c>
-      <c r="AZ33" t="n">
-        <v>8</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AZ33"/>
+      <c r="BA33"/>
+      <c r="BB33"/>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B34"/>
       <c r="C34"/>
       <c r="D34"/>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="F34"/>
       <c r="G34"/>
-      <c r="H34" t="n">
-        <v>6</v>
-      </c>
+      <c r="H34"/>
       <c r="I34"/>
-      <c r="J34" t="n">
-        <v>6</v>
-      </c>
+      <c r="J34"/>
       <c r="K34"/>
       <c r="L34" t="n">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="M34"/>
-      <c r="N34" t="n">
-        <v>5</v>
-      </c>
+      <c r="N34"/>
       <c r="O34"/>
-      <c r="P34"/>
+      <c r="P34" t="n">
+        <v>11</v>
+      </c>
       <c r="Q34"/>
       <c r="R34" t="n">
+        <v>8</v>
+      </c>
+      <c r="S34"/>
+      <c r="T34" t="n">
         <v>4</v>
       </c>
-      <c r="S34"/>
-      <c r="T34"/>
       <c r="U34"/>
-      <c r="V34"/>
+      <c r="V34" t="n">
+        <v>13</v>
+      </c>
       <c r="W34"/>
-      <c r="X34"/>
+      <c r="X34" t="n">
+        <v>10</v>
+      </c>
       <c r="Y34"/>
-      <c r="Z34"/>
+      <c r="Z34" t="n">
+        <v>8</v>
+      </c>
       <c r="AA34"/>
-      <c r="AB34"/>
+      <c r="AB34" t="n">
+        <v>18</v>
+      </c>
       <c r="AC34"/>
       <c r="AD34" t="n">
-        <v>2</v>
-      </c>
-      <c r="AE34" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF34"/>
+        <v>38</v>
+      </c>
+      <c r="AE34"/>
+      <c r="AF34" t="n">
+        <v>23</v>
+      </c>
       <c r="AG34"/>
-      <c r="AH34"/>
-      <c r="AI34"/>
+      <c r="AH34" t="n">
+        <v>18</v>
+      </c>
+      <c r="AI34" t="n">
+        <v>1</v>
+      </c>
       <c r="AJ34" t="n">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="AK34"/>
       <c r="AL34" t="n">
-        <v>2</v>
-      </c>
-      <c r="AM34" t="n">
-        <v>2</v>
-      </c>
-      <c r="AN34"/>
-      <c r="AO34"/>
-      <c r="AP34"/>
+        <v>32</v>
+      </c>
+      <c r="AM34"/>
+      <c r="AN34" t="n">
+        <v>23</v>
+      </c>
+      <c r="AO34" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP34" t="n">
+        <v>29</v>
+      </c>
       <c r="AQ34" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR34"/>
-      <c r="AS34" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT34"/>
+        <v>2</v>
+      </c>
+      <c r="AR34" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS34"/>
+      <c r="AT34" t="n">
+        <v>2</v>
+      </c>
       <c r="AU34"/>
       <c r="AV34" t="n">
         <v>1</v>
       </c>
       <c r="AW34" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX34"/>
-      <c r="AY34"/>
+        <v>5</v>
+      </c>
+      <c r="AX34" t="n">
+        <v>3</v>
+      </c>
+      <c r="AY34" t="n">
+        <v>3</v>
+      </c>
       <c r="AZ34"/>
-    </row>
-    <row r="35">
-      <c r="A35" t="s">
-        <v>85</v>
-      </c>
-      <c r="B35"/>
-      <c r="C35"/>
-      <c r="D35"/>
-      <c r="E35" t="n">
-        <v>16</v>
-      </c>
-      <c r="F35"/>
-      <c r="G35"/>
-      <c r="H35"/>
-      <c r="I35"/>
-      <c r="J35"/>
-      <c r="K35"/>
-      <c r="L35" t="n">
-        <v>27</v>
-      </c>
-      <c r="M35"/>
-      <c r="N35"/>
-      <c r="O35"/>
-      <c r="P35" t="n">
-        <v>11</v>
-      </c>
-      <c r="Q35"/>
-      <c r="R35" t="n">
-        <v>8</v>
-      </c>
-      <c r="S35"/>
-      <c r="T35" t="n">
-        <v>4</v>
-      </c>
-      <c r="U35"/>
-      <c r="V35" t="n">
-        <v>13</v>
-      </c>
-      <c r="W35"/>
-      <c r="X35" t="n">
-        <v>10</v>
-      </c>
-      <c r="Y35"/>
-      <c r="Z35" t="n">
-        <v>8</v>
-      </c>
-      <c r="AA35"/>
-      <c r="AB35" t="n">
-        <v>18</v>
-      </c>
-      <c r="AC35"/>
-      <c r="AD35" t="n">
-        <v>38</v>
-      </c>
-      <c r="AE35"/>
-      <c r="AF35" t="n">
-        <v>23</v>
-      </c>
-      <c r="AG35"/>
-      <c r="AH35" t="n">
-        <v>18</v>
-      </c>
-      <c r="AI35" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ35" t="n">
-        <v>24</v>
-      </c>
-      <c r="AK35"/>
-      <c r="AL35" t="n">
-        <v>32</v>
-      </c>
-      <c r="AM35"/>
-      <c r="AN35" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO35" t="n">
-        <v>2</v>
-      </c>
-      <c r="AP35" t="n">
-        <v>3</v>
-      </c>
-      <c r="AQ35"/>
-      <c r="AR35" t="n">
-        <v>2</v>
-      </c>
-      <c r="AS35"/>
-      <c r="AT35" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU35" t="n">
-        <v>5</v>
-      </c>
-      <c r="AV35" t="n">
-        <v>3</v>
-      </c>
-      <c r="AW35" t="n">
-        <v>3</v>
-      </c>
-      <c r="AX35"/>
-      <c r="AY35" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ35" t="n">
+      <c r="BA34" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB34" t="n">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
21st April 1st update
</commit_message>
<xml_diff>
--- a/covid19_data/excel/state/ncov19state_wide.xlsx
+++ b/covid19_data/excel/state/ncov19state_wide.xlsx
@@ -882,7 +882,9 @@
         <v>1</v>
       </c>
       <c r="AO3"/>
-      <c r="AP3"/>
+      <c r="AP3" t="n">
+        <v>1</v>
+      </c>
       <c r="AQ3"/>
       <c r="AR3"/>
       <c r="AS3"/>
@@ -1240,7 +1242,9 @@
         <v>10</v>
       </c>
       <c r="AO7"/>
-      <c r="AP7"/>
+      <c r="AP7" t="n">
+        <v>17</v>
+      </c>
       <c r="AQ7"/>
       <c r="AR7" t="n">
         <v>2</v>
@@ -1540,7 +1544,9 @@
       <c r="AO10" t="n">
         <v>6</v>
       </c>
-      <c r="AP10"/>
+      <c r="AP10" t="n">
+        <v>78</v>
+      </c>
       <c r="AQ10" t="n">
         <v>7</v>
       </c>
@@ -1727,7 +1733,7 @@
         <v>5</v>
       </c>
       <c r="AP12" t="n">
-        <v>108</v>
+        <v>196</v>
       </c>
       <c r="AQ12" t="n">
         <v>7</v>
@@ -2060,7 +2066,9 @@
         <v>13</v>
       </c>
       <c r="AO15"/>
-      <c r="AP15"/>
+      <c r="AP15" t="n">
+        <v>14</v>
+      </c>
       <c r="AQ15"/>
       <c r="AR15"/>
       <c r="AS15"/>
@@ -2162,7 +2170,9 @@
         <v>8</v>
       </c>
       <c r="AO16"/>
-      <c r="AP16"/>
+      <c r="AP16" t="n">
+        <v>1</v>
+      </c>
       <c r="AQ16"/>
       <c r="AR16"/>
       <c r="AS16"/>
@@ -2277,7 +2287,7 @@
       </c>
       <c r="AO17"/>
       <c r="AP17" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="AQ17" t="n">
         <v>5</v>
@@ -2418,7 +2428,9 @@
       <c r="AO18" t="n">
         <v>12</v>
       </c>
-      <c r="AP18"/>
+      <c r="AP18" t="n">
+        <v>6</v>
+      </c>
       <c r="AQ18" t="n">
         <v>12</v>
       </c>
@@ -2616,7 +2628,9 @@
       <c r="AO20" t="n">
         <v>4</v>
       </c>
-      <c r="AP20"/>
+      <c r="AP20" t="n">
+        <v>78</v>
+      </c>
       <c r="AQ20"/>
       <c r="AR20" t="n">
         <v>2</v>
@@ -2753,7 +2767,7 @@
         <v>4</v>
       </c>
       <c r="AP21" t="n">
-        <v>283</v>
+        <v>466</v>
       </c>
       <c r="AQ21" t="n">
         <v>12</v>
@@ -3051,7 +3065,7 @@
       <c r="AN25"/>
       <c r="AO25"/>
       <c r="AP25" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AQ25"/>
       <c r="AR25"/>
@@ -3224,7 +3238,9 @@
       <c r="AO27" t="n">
         <v>1</v>
       </c>
-      <c r="AP27"/>
+      <c r="AP27" t="n">
+        <v>1</v>
+      </c>
       <c r="AQ27" t="n">
         <v>10</v>
       </c>
@@ -3353,7 +3369,7 @@
         <v>8</v>
       </c>
       <c r="AP28" t="n">
-        <v>57</v>
+        <v>98</v>
       </c>
       <c r="AQ28" t="n">
         <v>7</v>
@@ -3476,7 +3492,9 @@
         <v>105</v>
       </c>
       <c r="AO29"/>
-      <c r="AP29"/>
+      <c r="AP29" t="n">
+        <v>43</v>
+      </c>
       <c r="AQ29" t="n">
         <v>3</v>
       </c>
@@ -3610,7 +3628,9 @@
       <c r="AO30" t="n">
         <v>3</v>
       </c>
-      <c r="AP30"/>
+      <c r="AP30" t="n">
+        <v>14</v>
+      </c>
       <c r="AQ30" t="n">
         <v>2</v>
       </c>
@@ -3808,7 +3828,9 @@
       <c r="AO32" t="n">
         <v>4</v>
       </c>
-      <c r="AP32"/>
+      <c r="AP32" t="n">
+        <v>84</v>
+      </c>
       <c r="AQ32" t="n">
         <v>4</v>
       </c>
@@ -3912,7 +3934,9 @@
         <v>2</v>
       </c>
       <c r="AO33"/>
-      <c r="AP33"/>
+      <c r="AP33" t="n">
+        <v>2</v>
+      </c>
       <c r="AQ33"/>
       <c r="AR33"/>
       <c r="AS33" t="n">

</xml_diff>